<commit_message>
fix: ajoute les colonnes 'Unités' des indicateurs de B5 dans le template d'export xlsx
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5DDCD2-460D-414B-AEAC-54A2F78F08B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CC38FC-5862-4BA6-B09F-69F0B34F3011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
   <si>
     <t/>
   </si>
@@ -958,30 +958,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -991,6 +967,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -998,6 +983,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1613,26 +1613,26 @@
       <c r="O1" s="67"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="45" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="45" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="50"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -1788,86 +1788,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="54" t="s">
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="51" t="s">
+      <c r="J2" s="47"/>
+      <c r="K2" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="51" t="s">
+      <c r="M2" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="51" t="s">
+      <c r="O2" s="47"/>
+      <c r="P2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="Q2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="45" t="s">
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="48"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -1889,16 +1889,16 @@
       <c r="J3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="52"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="58"/>
       <c r="N3" s="15" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="52"/>
+      <c r="P3" s="58"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -1938,11 +1938,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -1951,6 +1946,11 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1981,29 +1981,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="55" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="61" t="s">
@@ -2018,12 +2018,12 @@
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="60"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="48"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2177,21 +2177,21 @@
       <c r="O1" s="65"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="45" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="45" t="s">
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2239,23 +2239,23 @@
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1"/>
-    <col min="2" max="4" width="15.7109375" style="2"/>
-    <col min="5" max="5" width="15.7109375" style="14"/>
-    <col min="6" max="7" width="15.7109375" style="2"/>
-    <col min="8" max="8" width="15.7109375" style="12"/>
-    <col min="9" max="16384" width="15.7109375" style="2"/>
+    <col min="1" max="2" width="15.7109375" style="1"/>
+    <col min="3" max="5" width="15.7109375" style="2"/>
+    <col min="6" max="6" width="15.7109375" style="14"/>
+    <col min="7" max="9" width="15.7109375" style="2"/>
+    <col min="10" max="10" width="15.7109375" style="12"/>
+    <col min="11" max="16384" width="15.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="65" t="s">
         <v>108</v>
       </c>
@@ -2273,56 +2273,69 @@
       <c r="M1" s="65"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="45" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="48"/>
-    </row>
-    <row r="3" spans="1:15" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
+    </row>
+    <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D195" xr:uid="{08640288-E073-495F-B644-7C0538E8EB09}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E195" xr:uid="{08640288-E073-495F-B644-7C0538E8EB09}">
       <formula1>"OUI,NON"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A227 F4:F280" xr:uid="{9DBA5934-DC25-4318-BF4A-B23AEDD96D11}">
+      <formula1>"mètres carrés (m²),hectares (ha)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2369,11 +2382,11 @@
       <c r="O1" s="65"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="55" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2384,7 +2397,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2439,25 +2452,25 @@
       <c r="O1" s="65"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="48"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="50"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
@@ -2541,21 +2554,21 @@
       <c r="O1" s="66"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="45" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49" t="s">
+      <c r="H2" s="50"/>
+      <c r="I2" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2584,7 +2597,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="50"/>
+      <c r="I3" s="56"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -2642,11 +2655,11 @@
       <c r="O1" s="66"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="55" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2657,7 +2670,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="56"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>

</xml_diff>

<commit_message>
exporte B3 dans le template excel
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CC38FC-5862-4BA6-B09F-69F0B34F3011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C614CA2-E438-44B7-AB8D-9FBA4CACEE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
     <sheet name="B1" sheetId="7" r:id="rId2"/>
     <sheet name="B2" sheetId="2" r:id="rId3"/>
-    <sheet name="B4" sheetId="8" r:id="rId4"/>
-    <sheet name="B5" sheetId="17" r:id="rId5"/>
-    <sheet name="B6" sheetId="9" r:id="rId6"/>
-    <sheet name="B7" sheetId="10" r:id="rId7"/>
-    <sheet name="B8" sheetId="15" r:id="rId8"/>
-    <sheet name="B9" sheetId="11" r:id="rId9"/>
-    <sheet name="B10" sheetId="16" r:id="rId10"/>
-    <sheet name="B11" sheetId="14" r:id="rId11"/>
+    <sheet name="B3" sheetId="18" r:id="rId4"/>
+    <sheet name="B4" sheetId="8" r:id="rId5"/>
+    <sheet name="B5" sheetId="17" r:id="rId6"/>
+    <sheet name="B6" sheetId="9" r:id="rId7"/>
+    <sheet name="B7" sheetId="10" r:id="rId8"/>
+    <sheet name="B8" sheetId="15" r:id="rId9"/>
+    <sheet name="B9" sheetId="11" r:id="rId10"/>
+    <sheet name="B10" sheetId="16" r:id="rId11"/>
+    <sheet name="B11" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="138">
   <si>
     <t/>
   </si>
@@ -401,6 +402,63 @@
   </si>
   <si>
     <t>Situé à proximité d’une zone sensible</t>
+  </si>
+  <si>
+    <t>B3 - Énergie et émissions de gaz à effet de serre</t>
+  </si>
+  <si>
+    <t>Renouvelable</t>
+  </si>
+  <si>
+    <t>Non renouvelable</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Consommation d'électricité</t>
+  </si>
+  <si>
+    <t>Estimation des émissions brutes de gaz à effet de serre (GES)</t>
+  </si>
+  <si>
+    <t>Scope 1</t>
+  </si>
+  <si>
+    <t>Scope 2</t>
+  </si>
+  <si>
+    <t>Intensité GES</t>
+  </si>
+  <si>
+    <t>Consommation d'énergie par combustible</t>
+  </si>
+  <si>
+    <t>Autres combustibles</t>
+  </si>
+  <si>
+    <t>Consommation d'énergie totale</t>
+  </si>
+  <si>
+    <t>Type de combustible</t>
+  </si>
+  <si>
+    <t>État chimique</t>
+  </si>
+  <si>
+    <t>Renouvelable/Non renouvelable</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Énergie calculée</t>
+  </si>
+  <si>
+    <t>Énergie consommée</t>
+  </si>
+  <si>
+    <t>Consommation de combustibles</t>
   </si>
 </sst>
 </file>
@@ -888,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1041,6 +1099,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1570,6 +1643,77 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D36321D-28CF-4197-97E4-15B03B8FE828}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="56"/>
+    </row>
+    <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
+      <c r="E12" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C8CD-15EF-412F-8BDE-09F42DF51D25}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1577,7 +1721,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G3" sqref="G3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1697,7 +1841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2135,6 +2279,174 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E4342-D345-4F6D-8348-EF5BA58D69DD}">
+  <sheetPr>
+    <tabColor rgb="FFB8FEC9"/>
+  </sheetPr>
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1"/>
+    <col min="3" max="3" width="15.7109375" style="12"/>
+    <col min="4" max="8" width="15.7109375" style="2"/>
+    <col min="9" max="9" width="15.7109375" style="12"/>
+    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="2"/>
+    <col min="12" max="12" width="15.7109375" style="12"/>
+    <col min="13" max="14" width="15.7109375" style="2"/>
+    <col min="15" max="15" width="15.7109375" style="12"/>
+    <col min="16" max="17" width="15.7109375" style="1"/>
+    <col min="18" max="18" width="15.7109375" style="11"/>
+    <col min="19" max="19" width="15.7109375" style="12"/>
+    <col min="20" max="16384" width="15.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="50"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="D4" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="D2:O2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="J3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5692AB71-D55C-4890-A4C4-4497C431AAF2}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2234,14 +2546,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1C31A0-C7DA-43B1-B6AB-AA5BBBECAE63}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -2343,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBBB6-BAD2-4D62-996E-E16FA2533A1A}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2410,7 +2722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773AF20E-74BF-463C-9F61-BFE009D6FACB}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2511,7 +2823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD01D35-7DA1-4A19-9314-8C6D84659D0B}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -2613,75 +2925,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D36321D-28CF-4197-97E4-15B03B8FE828}">
-  <sheetPr>
-    <tabColor rgb="FFFEE7FC"/>
-  </sheetPr>
-  <dimension ref="A1:O12"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="12" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="56"/>
-    </row>
-    <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
-      <c r="E12" s="22"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: corrige l'export excel de B3 avec l'ajout des 2 colonnes supplémentaires
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C614CA2-E438-44B7-AB8D-9FBA4CACEE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28FF6C1-345A-438E-A1B3-20F76602A2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="B10" sheetId="16" r:id="rId11"/>
     <sheet name="B11" sheetId="14" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
   <si>
     <t/>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>Consommation de combustibles</t>
+  </si>
+  <si>
+    <t>Densité</t>
+  </si>
+  <si>
+    <t>Valeur Calorifique Nette (NCV)</t>
   </si>
 </sst>
 </file>
@@ -1013,9 +1019,36 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1025,56 +1058,44 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1099,21 +1120,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1613,11 +1619,11 @@
       </c>
     </row>
     <row r="11" spans="3:9" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="13" spans="3:9" ht="72.75" customHeight="1" x14ac:dyDescent="1.25">
       <c r="C13" s="8" t="s">
@@ -1663,30 +1669,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1697,7 +1703,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="56"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1738,45 +1744,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="48" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="48" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="56"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -1861,35 +1867,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="75" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1932,86 +1938,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="46" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="46" t="s">
+      <c r="N2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="47"/>
-      <c r="P2" s="57" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="51" t="s">
+      <c r="Q2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="48" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="50"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2033,16 +2039,16 @@
       <c r="J3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="58"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="58"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="53"/>
       <c r="N3" s="15" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="58"/>
+      <c r="P3" s="53"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2082,6 +2088,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2090,11 +2101,6 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2125,49 +2131,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2283,76 +2289,80 @@
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="1"/>
     <col min="3" max="3" width="15.7109375" style="12"/>
-    <col min="4" max="8" width="15.7109375" style="2"/>
-    <col min="9" max="9" width="15.7109375" style="12"/>
-    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="2"/>
-    <col min="12" max="12" width="15.7109375" style="12"/>
-    <col min="13" max="14" width="15.7109375" style="2"/>
-    <col min="15" max="15" width="15.7109375" style="12"/>
-    <col min="16" max="17" width="15.7109375" style="1"/>
-    <col min="18" max="18" width="15.7109375" style="11"/>
-    <col min="19" max="19" width="15.7109375" style="12"/>
-    <col min="20" max="16384" width="15.7109375" style="2"/>
+    <col min="4" max="10" width="15.7109375" style="2"/>
+    <col min="11" max="11" width="15.7109375" style="12"/>
+    <col min="12" max="12" width="15.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="2"/>
+    <col min="14" max="14" width="15.7109375" style="12"/>
+    <col min="15" max="16" width="15.7109375" style="2"/>
+    <col min="17" max="17" width="15.7109375" style="12"/>
+    <col min="18" max="19" width="15.7109375" style="1"/>
+    <col min="20" max="20" width="15.7109375" style="11"/>
+    <col min="21" max="21" width="15.7109375" style="12"/>
+    <col min="22" max="16384" width="15.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:21" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-    </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="49" t="s">
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="50"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="49"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>120</v>
       </c>
@@ -2362,38 +2372,40 @@
       <c r="C3" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76" t="s">
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="S3" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="25.5" x14ac:dyDescent="0.35">
       <c r="D4" s="16" t="s">
         <v>131</v>
       </c>
@@ -2404,42 +2416,48 @@
         <v>133</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="J4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="K4" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="M4" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="N4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="O4" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="P4" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="D2:O2"/>
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2470,40 +2488,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="48" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="48" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2568,41 +2586,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="48" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2675,30 +2693,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2709,7 +2727,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="56"/>
+      <c r="C3" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2745,44 +2763,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="48" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
@@ -2847,40 +2865,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="48" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="55" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="50" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2909,7 +2927,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="56"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>

</xml_diff>

<commit_message>
exporte l'exigence de publication C1 uniquement pour les rapports basés sur le module complet
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28FF6C1-345A-438E-A1B3-20F76602A2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735E571D-40C2-4565-870C-643C6B6F74EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
     <sheet name="B1" sheetId="7" r:id="rId2"/>
     <sheet name="B2" sheetId="2" r:id="rId3"/>
-    <sheet name="B3" sheetId="18" r:id="rId4"/>
-    <sheet name="B4" sheetId="8" r:id="rId5"/>
-    <sheet name="B5" sheetId="17" r:id="rId6"/>
-    <sheet name="B6" sheetId="9" r:id="rId7"/>
-    <sheet name="B7" sheetId="10" r:id="rId8"/>
-    <sheet name="B8" sheetId="15" r:id="rId9"/>
-    <sheet name="B9" sheetId="11" r:id="rId10"/>
-    <sheet name="B10" sheetId="16" r:id="rId11"/>
-    <sheet name="B11" sheetId="14" r:id="rId12"/>
+    <sheet name="C1" sheetId="19" r:id="rId4"/>
+    <sheet name="B3" sheetId="18" r:id="rId5"/>
+    <sheet name="B4" sheetId="8" r:id="rId6"/>
+    <sheet name="B5" sheetId="17" r:id="rId7"/>
+    <sheet name="B6" sheetId="9" r:id="rId8"/>
+    <sheet name="B7" sheetId="10" r:id="rId9"/>
+    <sheet name="B8" sheetId="15" r:id="rId10"/>
+    <sheet name="B9" sheetId="11" r:id="rId11"/>
+    <sheet name="B10" sheetId="16" r:id="rId12"/>
+    <sheet name="B11" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
   <si>
     <t/>
   </si>
@@ -465,6 +466,21 @@
   </si>
   <si>
     <t>Valeur Calorifique Nette (NCV)</t>
+  </si>
+  <si>
+    <t>Produits et services proposés</t>
+  </si>
+  <si>
+    <t>Marchés sur lesquels l'entreprise exerce ses activités</t>
+  </si>
+  <si>
+    <t>Principales relations d'affaires</t>
+  </si>
+  <si>
+    <t>Éléments clés liés aux enjeux de durabilité</t>
+  </si>
+  <si>
+    <t>C1 - Stratégie : modèle économique et initiatives liées à la durabilité</t>
   </si>
 </sst>
 </file>
@@ -1025,30 +1041,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,6 +1050,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1065,6 +1066,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1649,6 +1665,110 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD01D35-7DA1-4A19-9314-8C6D84659D0B}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="11" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="11.42578125" style="14"/>
+    <col min="8" max="8" width="11.42578125" style="2"/>
+    <col min="9" max="9" width="11.42578125" style="13"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+    </row>
+    <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="51"/>
+      <c r="I2" s="56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="57"/>
+    </row>
+    <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
+      <c r="E12" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D36321D-28CF-4197-97E4-15B03B8FE828}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1688,11 +1808,11 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="56" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1703,7 +1823,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1719,7 +1839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C8CD-15EF-412F-8BDE-09F42DF51D25}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1763,26 +1883,26 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="46" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="51"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -1847,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -1916,7 +2036,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1938,86 +2058,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="55" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="56"/>
-      <c r="P2" s="52" t="s">
+      <c r="O2" s="48"/>
+      <c r="P2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="46" t="s">
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2039,16 +2159,16 @@
       <c r="J3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="53"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="59"/>
       <c r="N3" s="15" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="53"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2088,11 +2208,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2101,6 +2216,11 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2114,8 +2234,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G10"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2131,29 +2251,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="62" t="s">
@@ -2168,12 +2288,12 @@
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="61"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="49"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2285,14 +2405,83 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EA4131-FF48-4CC6-914C-333C7103E886}">
+  <sheetPr>
+    <tabColor rgb="FFFFEDC3"/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" style="11" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="12"/>
+    <col min="5" max="16384" width="15.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+    </row>
+    <row r="2" spans="1:13" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="51"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E4342-D345-4F6D-8348-EF5BA58D69DD}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2334,11 +2523,11 @@
       <c r="U1" s="44"/>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="67" t="s">
         <v>137</v>
       </c>
@@ -2355,12 +2544,12 @@
       <c r="O2" s="68"/>
       <c r="P2" s="68"/>
       <c r="Q2" s="69"/>
-      <c r="R2" s="47" t="s">
+      <c r="R2" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="49"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2464,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5692AB71-D55C-4890-A4C4-4497C431AAF2}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2507,21 +2696,21 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="46" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2564,7 +2753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1C31A0-C7DA-43B1-B6AB-AA5BBBECAE63}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2607,20 +2796,20 @@
       <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="46" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2673,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBBB6-BAD2-4D62-996E-E16FA2533A1A}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2712,11 +2901,11 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="56" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2727,7 +2916,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2740,7 +2929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773AF20E-74BF-463C-9F61-BFE009D6FACB}">
   <sheetPr>
     <tabColor rgb="FFB8FEC9"/>
@@ -2782,25 +2971,25 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="46" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="49"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
@@ -2839,108 +3028,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD01D35-7DA1-4A19-9314-8C6D84659D0B}">
-  <sheetPr>
-    <tabColor rgb="FFFEE7FC"/>
-  </sheetPr>
-  <dimension ref="A1:O12"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="11" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="2"/>
-    <col min="7" max="7" width="11.42578125" style="14"/>
-    <col min="8" max="8" width="11.42578125" style="2"/>
-    <col min="9" max="9" width="11.42578125" style="13"/>
-    <col min="10" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-    </row>
-    <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="51"/>
-    </row>
-    <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
-      <c r="E12" s="22"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
exporte l'exigence de publication C9 dans l'export excel
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735E571D-40C2-4565-870C-643C6B6F74EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F491A2BB-3FD2-46AD-92BD-EA86694873AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="B9" sheetId="11" r:id="rId11"/>
     <sheet name="B10" sheetId="16" r:id="rId12"/>
     <sheet name="B11" sheetId="14" r:id="rId13"/>
+    <sheet name="C9" sheetId="20" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="147">
   <si>
     <t/>
   </si>
@@ -481,6 +482,12 @@
   </si>
   <si>
     <t>C1 - Stratégie : modèle économique et initiatives liées à la durabilité</t>
+  </si>
+  <si>
+    <t>C9 - Ratio de mixité au sein de l’organe de gouvernance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio de mixité au sein de l’organe de gouvernance </t>
   </si>
 </sst>
 </file>
@@ -1041,6 +1048,30 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1050,15 +1081,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1066,21 +1088,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1707,21 +1714,21 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="56" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="50" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1750,7 +1757,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="57"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1808,11 +1815,11 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1823,7 +1830,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1883,26 +1890,26 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="57"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -1975,7 +1982,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2022,6 +2029,60 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
+  <sheetPr>
+    <tabColor rgb="FFE8EDFF"/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="11" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2058,86 +2119,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="47" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="58" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="M2" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="47" t="s">
+      <c r="N2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="58" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="52" t="s">
+      <c r="Q2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="49" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2159,16 +2220,16 @@
       <c r="J3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="59"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="53"/>
       <c r="N3" s="15" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="59"/>
+      <c r="P3" s="53"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2208,6 +2269,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2216,11 +2282,6 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2251,29 +2312,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="62" t="s">
@@ -2288,12 +2349,12 @@
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="61"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2411,7 +2472,7 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+    <sheetView zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -2424,41 +2485,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="50" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2523,11 +2584,11 @@
       <c r="U1" s="44"/>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="67" t="s">
         <v>137</v>
       </c>
@@ -2544,12 +2605,12 @@
       <c r="O2" s="68"/>
       <c r="P2" s="68"/>
       <c r="Q2" s="69"/>
-      <c r="R2" s="50" t="s">
+      <c r="R2" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="51"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2696,21 +2757,21 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="49" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2796,20 +2857,20 @@
       <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="49" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2901,11 +2962,11 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2916,7 +2977,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2971,25 +3032,25 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="49" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="57"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
exporte les indicateurs de C6 dans l'export excel vsme
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F491A2BB-3FD2-46AD-92BD-EA86694873AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C802B04-1DD5-4BD9-85E5-E6785260DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -24,9 +24,10 @@
     <sheet name="B7" sheetId="10" r:id="rId9"/>
     <sheet name="B8" sheetId="15" r:id="rId10"/>
     <sheet name="B9" sheetId="11" r:id="rId11"/>
-    <sheet name="B10" sheetId="16" r:id="rId12"/>
-    <sheet name="B11" sheetId="14" r:id="rId13"/>
-    <sheet name="C9" sheetId="20" r:id="rId14"/>
+    <sheet name="C6" sheetId="21" r:id="rId12"/>
+    <sheet name="B10" sheetId="16" r:id="rId13"/>
+    <sheet name="B11" sheetId="14" r:id="rId14"/>
+    <sheet name="C9" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="156">
   <si>
     <t/>
   </si>
@@ -488,6 +489,33 @@
   </si>
   <si>
     <t xml:space="preserve">Ratio de mixité au sein de l’organe de gouvernance </t>
+  </si>
+  <si>
+    <t>Politiques en matière de droits de l’homme</t>
+  </si>
+  <si>
+    <t>La politique de l'entreprise couvre-t-elle le travail des enfants ?</t>
+  </si>
+  <si>
+    <t>La politique de l'entreprise couvre-t-elle le travail forcé ?</t>
+  </si>
+  <si>
+    <t>La politique de l'entreprise couvre-t-elle la traite des êtres humains ?</t>
+  </si>
+  <si>
+    <t>La politique de l'entreprise couvre-t-elle la discrimination ?</t>
+  </si>
+  <si>
+    <t>La politique de l'entreprise couvre-t-elle la prévention des accidents ?</t>
+  </si>
+  <si>
+    <t>Autres thèmes couverts par la politique de l'entreprise</t>
+  </si>
+  <si>
+    <t>Mécanisme de traitement des plaintes pour le personnel</t>
+  </si>
+  <si>
+    <t>C6 - Informations complémentaires sur les effectifs de l'entreprise – Politiques et procédures en matière de droits de l’homme</t>
   </si>
 </sst>
 </file>
@@ -1048,18 +1076,36 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1070,24 +1116,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1714,21 +1742,21 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="56" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1757,7 +1785,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="51"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1815,11 +1843,11 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="56" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1830,7 +1858,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1847,6 +1875,105 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C465E33-2082-481B-93DA-B52297D05DCF}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="12" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="56" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="89.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="12" spans="1:19" ht="72.75" x14ac:dyDescent="1.25">
+      <c r="I12" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CDC385A0-B5FD-401E-93AD-22065DF458B9}">
+      <formula1>"Oui;Non"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:E6 G4:G6" xr:uid="{7DBAC362-146C-4B4C-AD0A-4C9EC713BD69}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C8CD-15EF-412F-8BDE-09F42DF51D25}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1890,26 +2017,26 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="46" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="51"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -1974,7 +2101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2035,14 +2162,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2119,86 +2246,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="55" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="56"/>
-      <c r="P2" s="52" t="s">
+      <c r="O2" s="48"/>
+      <c r="P2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="46" t="s">
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2220,16 +2347,16 @@
       <c r="J3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="53"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="59"/>
       <c r="N3" s="15" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="53"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2269,11 +2396,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2282,6 +2404,11 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2296,7 +2423,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2312,29 +2439,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="62" t="s">
@@ -2349,12 +2476,12 @@
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="61"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="49"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2485,41 +2612,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="55" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="56" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2584,11 +2711,11 @@
       <c r="U1" s="44"/>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="67" t="s">
         <v>137</v>
       </c>
@@ -2605,12 +2732,12 @@
       <c r="O2" s="68"/>
       <c r="P2" s="68"/>
       <c r="Q2" s="69"/>
-      <c r="R2" s="47" t="s">
+      <c r="R2" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="49"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2757,21 +2884,21 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="46" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="46" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2857,20 +2984,20 @@
       <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="46" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2962,11 +3089,11 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="56" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2977,7 +3104,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3032,25 +3159,25 @@
       <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="46" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="49"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
exporte les indicateurs de C8 dans l'export excel
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C802B04-1DD5-4BD9-85E5-E6785260DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4356DC7F-9599-451D-9B0D-D47648DF4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="C6" sheetId="21" r:id="rId12"/>
     <sheet name="B10" sheetId="16" r:id="rId13"/>
     <sheet name="B11" sheetId="14" r:id="rId14"/>
-    <sheet name="C9" sheetId="20" r:id="rId15"/>
+    <sheet name="C8" sheetId="22" r:id="rId15"/>
+    <sheet name="C9" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="166">
   <si>
     <t/>
   </si>
@@ -516,6 +517,36 @@
   </si>
   <si>
     <t>C6 - Informations complémentaires sur les effectifs de l'entreprise – Politiques et procédures en matière de droits de l’homme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu des armes controversées </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu du tabac </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu des combustibles fossiles du charbon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu des combustibles fossiles du pétrole </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu des combustibles fossiles du gaz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires issu des pesticides et produits agrochimiques </t>
+  </si>
+  <si>
+    <t>Exclusion des indices de référence de l’Union Européenne (« Accord de Paris »)</t>
+  </si>
+  <si>
+    <t>Chiffre d’affaires dans certains secteurs sensibles</t>
+  </si>
+  <si>
+    <t>C8 - Recettes de certains secteurs et exclusion des indices de référence de l'UE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total du chiffre d’affaires issu des combustibles fossiles (charbon, pétrole, gaz) </t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1153,9 +1184,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1881,8 +1909,8 @@
   </sheetPr>
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G2" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1981,7 +2009,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:I4"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1998,23 +2026,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
@@ -2109,7 +2137,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2121,35 +2149,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="74"/>
-      <c r="B3" s="76"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2163,6 +2191,96 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA71AC8-3159-49A5-B6FC-4FA1DF3F7E26}">
+  <sheetPr>
+    <tabColor rgb="FFE8EDFF"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K14" sqref="K13:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1"/>
+    <col min="2" max="6" width="15.7109375" style="2"/>
+    <col min="7" max="7" width="15.7109375" style="12"/>
+    <col min="8" max="8" width="18.140625" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="15.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="63.75" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H6" xr:uid="{B7229605-3AFC-4A61-911C-7A7A7D3FA5D1}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2170,7 +2288,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2181,30 +2299,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="74"/>
+      <c r="A3" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
exporte les indicateurs de C5 dans l'export excel vsme
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4356DC7F-9599-451D-9B0D-D47648DF4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01CDB67-A783-41DA-882E-30A946A65F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -24,11 +24,12 @@
     <sheet name="B7" sheetId="10" r:id="rId9"/>
     <sheet name="B8" sheetId="15" r:id="rId10"/>
     <sheet name="B9" sheetId="11" r:id="rId11"/>
-    <sheet name="C6" sheetId="21" r:id="rId12"/>
-    <sheet name="B10" sheetId="16" r:id="rId13"/>
-    <sheet name="B11" sheetId="14" r:id="rId14"/>
-    <sheet name="C8" sheetId="22" r:id="rId15"/>
-    <sheet name="C9" sheetId="20" r:id="rId16"/>
+    <sheet name="B10" sheetId="16" r:id="rId12"/>
+    <sheet name="C5" sheetId="23" r:id="rId13"/>
+    <sheet name="C6" sheetId="21" r:id="rId14"/>
+    <sheet name="B11" sheetId="14" r:id="rId15"/>
+    <sheet name="C8" sheetId="22" r:id="rId16"/>
+    <sheet name="C9" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="173">
   <si>
     <t/>
   </si>
@@ -547,6 +548,27 @@
   </si>
   <si>
     <t xml:space="preserve">Total du chiffre d’affaires issu des combustibles fossiles (charbon, pétrole, gaz) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de salariés hommes occupant des postes de direction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de salariées femmes occupant des postes de direction </t>
+  </si>
+  <si>
+    <t>Ratio femmes/hommes au niveau de l'encadrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total des travailleurs indépendants sans personnel qui travaillent exclusivement pour l’entreprise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total des travailleurs temporaires mis à disposition par des entreprises exerçant principalement des activités liées à l’emploi </t>
+  </si>
+  <si>
+    <t>Travailleurs indépendants et salariés temporaires</t>
+  </si>
+  <si>
+    <t>C5 - Caractéristiques supplémentaires (générales) des effectifs</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1103,6 +1125,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1274,10 +1302,10 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFEDC3"/>
       <color rgb="FFE8EDFF"/>
       <color rgb="FFFEE7FC"/>
       <color rgb="FFB8FEC9"/>
-      <color rgb="FFFFEDC3"/>
       <color rgb="FF8F7C0D"/>
     </mruColors>
   </colors>
@@ -1698,11 +1726,11 @@
       </c>
     </row>
     <row r="11" spans="3:9" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
     </row>
     <row r="13" spans="3:9" ht="72.75" customHeight="1" x14ac:dyDescent="1.25">
       <c r="C13" s="8" t="s">
@@ -1751,40 +1779,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="56" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="58" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1813,7 +1841,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="57"/>
+      <c r="I3" s="59"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1852,30 +1880,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="58" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1886,7 +1914,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1903,105 +1931,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C465E33-2082-481B-93DA-B52297D05DCF}">
-  <sheetPr>
-    <tabColor rgb="FFFEE7FC"/>
-  </sheetPr>
-  <dimension ref="A1:S12"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="5" width="11.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="12" customWidth="1"/>
-    <col min="8" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="89.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="57"/>
-    </row>
-    <row r="12" spans="1:19" ht="72.75" x14ac:dyDescent="1.25">
-      <c r="I12" s="22"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:G3"/>
-  </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CDC385A0-B5FD-401E-93AD-22065DF458B9}">
-      <formula1>"Oui;Non"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:E6 G4:G6" xr:uid="{7DBAC362-146C-4B4C-AD0A-4C9EC713BD69}">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C8CD-15EF-412F-8BDE-09F42DF51D25}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -2026,45 +1955,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="57"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -2129,7 +2058,192 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F62B1A-C319-4701-AD63-7BD53F525CF6}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+    </row>
+    <row r="2" spans="1:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="53"/>
+    </row>
+    <row r="3" spans="1:15" ht="114.75" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B6 D4:D6" xr:uid="{ECF2B690-DE8C-4553-9209-BA2AD45D05AF}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C5 E4:E5" xr:uid="{AA26721B-E646-42C7-B623-10508B421A95}">
+      <formula1>"Oui;Non"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C465E33-2082-481B-93DA-B52297D05DCF}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="12" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="58" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="89.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="59"/>
+    </row>
+    <row r="12" spans="1:19" ht="72.75" x14ac:dyDescent="1.25">
+      <c r="I12" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CDC385A0-B5FD-401E-93AD-22065DF458B9}">
+      <formula1>"Oui;Non"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:E6 G4:G6" xr:uid="{7DBAC362-146C-4B4C-AD0A-4C9EC713BD69}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2149,35 +2263,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="76" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="75"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2190,14 +2304,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA71AC8-3159-49A5-B6FC-4FA1DF3F7E26}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="K14" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
@@ -2211,32 +2325,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="55" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="57" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2262,7 +2376,7 @@
       <c r="G3" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="51"/>
+      <c r="H3" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2280,7 +2394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2299,30 +2413,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
+      <c r="A3" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2341,8 +2455,8 @@
   </sheetPr>
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A4" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2360,90 +2474,92 @@
     <col min="17" max="17" width="15.7109375" style="14"/>
     <col min="18" max="22" width="15.7109375" style="2"/>
     <col min="23" max="23" width="15.7109375" style="12"/>
-    <col min="24" max="16384" width="15.7109375" style="2"/>
+    <col min="24" max="27" width="15.7109375" style="2"/>
+    <col min="28" max="28" width="15.7109375" style="12"/>
+    <col min="29" max="16384" width="15.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="47" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="58" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="M2" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="47" t="s">
+      <c r="N2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="58" t="s">
+      <c r="O2" s="50"/>
+      <c r="P2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="52" t="s">
+      <c r="Q2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="49" t="s">
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="53"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2459,22 +2575,22 @@
       <c r="H3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="15" t="s">
+      <c r="K3" s="61"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="59"/>
+      <c r="P3" s="61"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2508,7 +2624,7 @@
       <c r="AA3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AB3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2557,49 +2673,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="61"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2730,41 +2846,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
     </row>
     <row r="2" spans="1:13" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="58" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2808,54 +2924,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
       <c r="R1" s="44"/>
       <c r="S1" s="44"/>
       <c r="T1" s="44"/>
       <c r="U1" s="44"/>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="67" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="50" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="51"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2867,26 +2983,26 @@
       <c r="C3" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66" t="s">
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66" t="s">
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
       <c r="R3" s="15" t="s">
         <v>125</v>
       </c>
@@ -2983,40 +3099,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="49" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3081,41 +3197,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="49" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3188,30 +3304,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="58" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3222,7 +3338,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3258,44 +3374,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="49" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="57"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
exporte les indicateurs de C7 dans l'export excel vsme
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01CDB67-A783-41DA-882E-30A946A65F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9B35E-26DD-41A5-AB02-16B6713B0860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="B10" sheetId="16" r:id="rId12"/>
     <sheet name="C5" sheetId="23" r:id="rId13"/>
     <sheet name="C6" sheetId="21" r:id="rId14"/>
-    <sheet name="B11" sheetId="14" r:id="rId15"/>
-    <sheet name="C8" sheetId="22" r:id="rId16"/>
-    <sheet name="C9" sheetId="20" r:id="rId17"/>
+    <sheet name="C7" sheetId="24" r:id="rId15"/>
+    <sheet name="B11" sheetId="14" r:id="rId16"/>
+    <sheet name="C8" sheetId="22" r:id="rId17"/>
+    <sheet name="C9" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="182">
   <si>
     <t/>
   </si>
@@ -569,6 +570,33 @@
   </si>
   <si>
     <t>C5 - Caractéristiques supplémentaires (générales) des effectifs</t>
+  </si>
+  <si>
+    <t>Incidents graves en matière de droits de l’homme au sein du personnel</t>
+  </si>
+  <si>
+    <t>L’entreprise a-t-elle confirmé des incidents graves au sein de son personnel liés au travail des enfants ?</t>
+  </si>
+  <si>
+    <t>L’entreprise a-t-elle confirmé des incidents graves au sein de son personnel liés au travail forcé ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’entreprise a-t-elle confirmé des incidents graves au sein de son personnel liés à la traite des êtres humains ? </t>
+  </si>
+  <si>
+    <t>L’entreprise a-t-elle confirmé des incidents graves au sein de son personnel liés à la discrimination ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description des actions mises en oeuvre pour gérer les indidents confirmés </t>
+  </si>
+  <si>
+    <t>Autres thèmes concernant des indidents graves confirmés relatifs aux droits de l’homme</t>
+  </si>
+  <si>
+    <t>Incidents graves en matière de droits de l’homme dans la chaîne de valeur et auprès des parties prenantes externes</t>
+  </si>
+  <si>
+    <t>C7 - Incidents graves en matière de droits de l’homme</t>
   </si>
 </sst>
 </file>
@@ -1135,6 +1163,30 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,15 +1196,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,21 +1203,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1798,21 +1826,21 @@
       <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="51" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="58" t="s">
+      <c r="H2" s="50"/>
+      <c r="I2" s="52" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1841,7 +1869,7 @@
       <c r="H3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="59"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1899,11 +1927,11 @@
       <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="52" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1914,7 +1942,7 @@
       <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="59"/>
+      <c r="C3" s="53"/>
     </row>
     <row r="12" spans="1:15" ht="72.75" x14ac:dyDescent="1.25">
       <c r="E12" s="22"/>
@@ -1974,26 +2002,26 @@
       <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="51" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="51" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="59"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="15" t="s">
         <v>95</v>
       </c>
@@ -2065,7 +2093,7 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -2098,15 +2126,15 @@
       <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="51" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="114.75" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -2188,15 +2216,15 @@
       <c r="S1" s="73"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="58" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="52" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2219,7 +2247,7 @@
       <c r="F3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="12" spans="1:19" ht="72.75" x14ac:dyDescent="1.25">
       <c r="I12" s="22"/>
@@ -2244,6 +2272,105 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D0B7EC-F23C-48FB-98BB-3AFB974D2AA9}">
+  <sheetPr>
+    <tabColor rgb="FFFEE7FC"/>
+  </sheetPr>
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="12" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="21" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="127.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="53"/>
+    </row>
+    <row r="12" spans="1:19" ht="72.75" x14ac:dyDescent="1.25">
+      <c r="I12" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:D6" xr:uid="{1B2DE9D8-64C5-4348-ADE4-E77390153108}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{3798302E-94F3-4507-9943-C3A3D9E5FD92}">
+      <formula1>"Oui;Non"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2304,7 +2431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA71AC8-3159-49A5-B6FC-4FA1DF3F7E26}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2341,16 +2468,16 @@
       <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="57" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2376,7 +2503,7 @@
       <c r="G3" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="53"/>
+      <c r="H3" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2394,7 +2521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2480,86 +2607,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
     </row>
     <row r="2" spans="1:28" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="49" t="s">
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="60" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="L2" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="N2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="60" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="54" t="s">
+      <c r="Q2" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="51" t="s">
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="53"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="50"/>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2581,16 +2708,16 @@
       <c r="J3" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="61"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="55"/>
       <c r="N3" s="45" t="s">
         <v>74</v>
       </c>
       <c r="O3" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="61"/>
+      <c r="P3" s="55"/>
       <c r="Q3" s="17" t="s">
         <v>72</v>
       </c>
@@ -2630,6 +2757,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2638,11 +2770,6 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2673,29 +2800,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="52" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="64" t="s">
@@ -2710,12 +2837,12 @@
     </row>
     <row r="3" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:15" ht="48" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="25" t="s">
@@ -2846,41 +2973,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="1:13" s="19" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="52" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2945,11 +3072,11 @@
       <c r="U1" s="44"/>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="69" t="s">
         <v>137</v>
       </c>
@@ -2966,12 +3093,12 @@
       <c r="O2" s="70"/>
       <c r="P2" s="70"/>
       <c r="Q2" s="71"/>
-      <c r="R2" s="52" t="s">
+      <c r="R2" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="53"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="50"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3118,21 +3245,21 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="51" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="51" t="s">
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3218,20 +3345,20 @@
       <c r="Q1" s="72"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="51" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3323,11 +3450,11 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="52" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3338,7 +3465,7 @@
       <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="59"/>
+      <c r="C3" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3393,25 +3520,25 @@
       <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="51" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.35">
-      <c r="A3" s="59"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
exporte les indicateurs de C4 dans le fichier excel
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9B35E-26DD-41A5-AB02-16B6713B0860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C032B9-A9CA-4337-A9EE-CC37BC8FCA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;&gt; " sheetId="3" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="B5" sheetId="17" r:id="rId7"/>
     <sheet name="B6" sheetId="9" r:id="rId8"/>
     <sheet name="B7" sheetId="10" r:id="rId9"/>
-    <sheet name="B8" sheetId="15" r:id="rId10"/>
-    <sheet name="B9" sheetId="11" r:id="rId11"/>
-    <sheet name="B10" sheetId="16" r:id="rId12"/>
-    <sheet name="C5" sheetId="23" r:id="rId13"/>
-    <sheet name="C6" sheetId="21" r:id="rId14"/>
-    <sheet name="C7" sheetId="24" r:id="rId15"/>
-    <sheet name="B11" sheetId="14" r:id="rId16"/>
-    <sheet name="C8" sheetId="22" r:id="rId17"/>
-    <sheet name="C9" sheetId="20" r:id="rId18"/>
+    <sheet name="C4" sheetId="25" r:id="rId10"/>
+    <sheet name="B8" sheetId="15" r:id="rId11"/>
+    <sheet name="B9" sheetId="11" r:id="rId12"/>
+    <sheet name="B10" sheetId="16" r:id="rId13"/>
+    <sheet name="C5" sheetId="23" r:id="rId14"/>
+    <sheet name="C6" sheetId="21" r:id="rId15"/>
+    <sheet name="C7" sheetId="24" r:id="rId16"/>
+    <sheet name="B11" sheetId="14" r:id="rId17"/>
+    <sheet name="C8" sheetId="22" r:id="rId18"/>
+    <sheet name="C9" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="193">
   <si>
     <t/>
   </si>
@@ -597,6 +598,39 @@
   </si>
   <si>
     <t>C7 - Incidents graves en matière de droits de l’homme</t>
+  </si>
+  <si>
+    <t>Aléas et risques climatiques recensés</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Méthode d'évaluation </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horizon temporel </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actions d’adaptation entreprises </t>
+  </si>
+  <si>
+    <t>Impacts financiers potentiels des risques climatiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ce risque a-t-il des impacts financiers potentiels ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description des impacts financiers potentiels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Niveau de risque </t>
+  </si>
+  <si>
+    <t>C4 - Risques climatiques</t>
+  </si>
+  <si>
+    <t>N° du risque</t>
   </si>
 </sst>
 </file>
@@ -1784,6 +1818,119 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD57197-9ADC-43C0-B70E-801EE1BD86F4}">
+  <sheetPr>
+    <tabColor rgb="FFB8FEC9"/>
+  </sheetPr>
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="15.7109375" style="1"/>
+    <col min="4" max="5" width="15.7109375" style="2"/>
+    <col min="6" max="6" width="15.7109375" style="14"/>
+    <col min="7" max="8" width="15.7109375" style="2"/>
+    <col min="9" max="9" width="15.7109375" style="12"/>
+    <col min="10" max="16384" width="15.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="20" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
+    </row>
+    <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B227" xr:uid="{60BE6B91-29AF-41C7-B3A4-C4179A88EB71}">
+      <formula1>"mètres carrés (m²),hectares (ha)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E1048576" xr:uid="{AD7C7AAC-4515-4F38-AACF-A38E6B99C9CF}">
+      <formula1>"OUI,NON"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{29B113A3-BA67-47E6-8B8A-E2219ADE32EA}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1048576 I4 D4:D1048576" xr:uid="{409DDD9F-A932-41BF-BED3-9D409CF955FD}">
+      <formula1>"Court terme, Moyen terme, Long terme"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H1048576" xr:uid="{08B2E6BA-9233-4696-B15F-4D1D036C4550}">
+      <formula1>"Elevé,Moyen,Faible"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD01D35-7DA1-4A19-9314-8C6D84659D0B}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1887,7 +2034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D36321D-28CF-4197-97E4-15B03B8FE828}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -1958,7 +2105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8767C8CD-15EF-412F-8BDE-09F42DF51D25}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -2086,7 +2233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F62B1A-C319-4701-AD63-7BD53F525CF6}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -2172,7 +2319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C465E33-2082-481B-93DA-B52297D05DCF}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
@@ -2271,14 +2418,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D0B7EC-F23C-48FB-98BB-3AFB974D2AA9}">
   <sheetPr>
     <tabColor rgb="FFFEE7FC"/>
   </sheetPr>
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2370,7 +2517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E0E35-59BE-44D0-9FD8-FA3A89A617DC}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2431,7 +2578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA71AC8-3159-49A5-B6FC-4FA1DF3F7E26}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2521,7 +2668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD13986-9BC7-428C-BEF7-5E284E22308C}">
   <sheetPr>
     <tabColor rgb="FFE8EDFF"/>
@@ -2582,8 +2729,8 @@
   </sheetPr>
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView topLeftCell="O1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3029,8 +3176,8 @@
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3210,7 +3357,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3310,7 +3457,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fix: corrige l'onglet C4 du template d'export excel VSME
</commit_message>
<xml_diff>
--- a/impact/vsme/xlsx/VSME.xlsx
+++ b/impact/vsme/xlsx/VSME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmonteiro-de-mac-adc\Desktop\ancien bureau\Fichier\CSRD\Tableau ESRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C032B9-A9CA-4337-A9EE-CC37BC8FCA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F3BE4-E26B-4DE8-B69D-7530A0D7FF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1908,13 +1908,7 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:I2"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B227" xr:uid="{60BE6B91-29AF-41C7-B3A4-C4179A88EB71}">
-      <formula1>"mètres carrés (m²),hectares (ha)"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E1048576" xr:uid="{AD7C7AAC-4515-4F38-AACF-A38E6B99C9CF}">
-      <formula1>"OUI,NON"</formula1>
-    </dataValidation>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{29B113A3-BA67-47E6-8B8A-E2219ADE32EA}">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>

</xml_diff>